<commit_message>
Ví dụ về cách ghi thành tích.
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>BẢNG VÀNG THÀNH TÍCH</t>
   </si>
@@ -34,6 +34,27 @@
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Lê Văn Long</t>
+  </si>
+  <si>
+    <t>16/04</t>
+  </si>
+  <si>
+    <t>Project plan</t>
+  </si>
+  <si>
+    <t>Risk list</t>
+  </si>
+  <si>
+    <t>Võ Ngọc Tuyết Phượng</t>
+  </si>
+  <si>
+    <t>Bổ sung risk list</t>
+  </si>
+  <si>
+    <t>Ví dụ</t>
   </si>
 </sst>
 </file>
@@ -106,9 +127,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -119,6 +137,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,280 +438,300 @@
   <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>7</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>8</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>10</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>11</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>12</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>13</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>14</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>15</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>16</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>17</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>18</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>19</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>20</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>21</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>22</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>23</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>24</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>25</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
0712118 - Nguyen Le Hoang Dung Tao co so du lieu
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>BẢNG VÀNG THÀNH TÍCH</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Ví dụ</t>
+  </si>
+  <si>
+    <t>Nguyễn Lê Hoàng Dũng</t>
+  </si>
+  <si>
+    <t>Tạo cơ sở dữ liệu</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -141,6 +147,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +452,7 @@
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
@@ -539,9 +546,15 @@
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="8">
+        <v>40299</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7">

</xml_diff>

<commit_message>
Sửa đổi BangVangThanhTich.xlsx cho phù hợp với quy định mới
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>BẢNG VÀNG THÀNH TÍCH</t>
   </si>
@@ -24,50 +24,129 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Ngày</t>
-  </si>
-  <si>
     <t>Họ tên</t>
   </si>
   <si>
-    <t>Thành tích</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
     <t>Lê Văn Long</t>
   </si>
   <si>
-    <t>16/04</t>
-  </si>
-  <si>
-    <t>Project plan</t>
-  </si>
-  <si>
-    <t>Risk list</t>
-  </si>
-  <si>
     <t>Võ Ngọc Tuyết Phượng</t>
   </si>
   <si>
-    <t>Bổ sung risk list</t>
-  </si>
-  <si>
-    <t>Ví dụ</t>
-  </si>
-  <si>
     <t>Nguyễn Lê Hoàng Dũng</t>
   </si>
   <si>
-    <t>Tạo cơ sở dữ liệu</t>
+    <t>Nguyễn Toàn Nhân</t>
+  </si>
+  <si>
+    <t>Huỳnh Di Nguyên</t>
+  </si>
+  <si>
+    <t>Trần Đại Nghĩa</t>
+  </si>
+  <si>
+    <t>Hồ Thái Hoàng</t>
+  </si>
+  <si>
+    <t>Trương Hoàng Sơn</t>
+  </si>
+  <si>
+    <t>Trần Thị Mộng Kiều</t>
+  </si>
+  <si>
+    <t>Phan Viết Huy</t>
+  </si>
+  <si>
+    <t>Vũ Thị Ngọc Nhi</t>
+  </si>
+  <si>
+    <t>Đỗ Việt Dũng</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Anh</t>
+  </si>
+  <si>
+    <t>Nguyễn Tiến Đạt</t>
+  </si>
+  <si>
+    <t>Tăng Phương Quý</t>
+  </si>
+  <si>
+    <t>Lê Nguyễn Hoài Thu</t>
+  </si>
+  <si>
+    <t>Nguyễn Phan Thanh Trúc</t>
+  </si>
+  <si>
+    <t>Võ Thị Mỹ Hạnh</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Ngọc Trâm</t>
+  </si>
+  <si>
+    <t>Phan Hoàng Sơn</t>
+  </si>
+  <si>
+    <t>Trần Quang Quốc Anh</t>
+  </si>
+  <si>
+    <t>Nguyễn Mạnh Cường</t>
+  </si>
+  <si>
+    <t>Cao Hoàng Phúc An</t>
+  </si>
+  <si>
+    <t>Lê Trọng Cần</t>
+  </si>
+  <si>
+    <t>MSSV</t>
+  </si>
+  <si>
+    <t>Tổng điểm</t>
+  </si>
+  <si>
+    <t>Nhóm</t>
+  </si>
+  <si>
+    <t>ĐG lần 2</t>
+  </si>
+  <si>
+    <t>ĐG lần 3</t>
+  </si>
+  <si>
+    <t>ĐG lần 4</t>
+  </si>
+  <si>
+    <t>ĐG lần 
+(05/05)</t>
+  </si>
+  <si>
+    <t>ĐG lần 5</t>
+  </si>
+  <si>
+    <t>ĐG lần 6</t>
+  </si>
+  <si>
+    <t>ĐG lần 7</t>
+  </si>
+  <si>
+    <t>ĐG lần 8</t>
+  </si>
+  <si>
+    <t>ĐG lần 9</t>
+  </si>
+  <si>
+    <t>ĐG lần 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0000000"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,8 +167,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +194,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -126,28 +224,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -451,304 +632,731 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="14" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="5" spans="1:15" s="21" customFormat="1" ht="33" customHeight="1">
+      <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="E5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16.5" customHeight="1">
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="13">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5">
+        <v>712312</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="E6" s="3">
+        <f>100 + SUM(F6:AZ6)</f>
+        <v>100</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" customHeight="1">
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="7">
+        <v>712308</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="E7" s="3">
+        <f t="shared" ref="E7:E29" si="0">100 + SUM(F7:AZ7)</f>
+        <v>100</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" ht="16.5" customHeight="1">
       <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="B8" s="14"/>
+      <c r="C8" s="7">
+        <v>712303</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1">
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="8">
-        <v>40299</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="B9" s="14"/>
+      <c r="C9" s="7">
+        <v>712181</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" customHeight="1">
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="B10" s="15"/>
+      <c r="C10" s="7">
+        <v>712372</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="A11" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="B11" s="13">
+        <v>17</v>
+      </c>
+      <c r="C11" s="9">
+        <v>712255</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" ht="16.5" customHeight="1">
       <c r="A12" s="3">
         <v>7</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="B12" s="14"/>
+      <c r="C12" s="11">
+        <v>712229</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" customHeight="1">
       <c r="A13" s="3">
         <v>8</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="B13" s="14"/>
+      <c r="C13" s="11">
+        <v>712201</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" customHeight="1">
       <c r="A14" s="3">
         <v>9</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="B14" s="14"/>
+      <c r="C14" s="11">
+        <v>712314</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" ht="16.5" customHeight="1">
       <c r="A15" s="3">
         <v>10</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="B15" s="15"/>
+      <c r="C15" s="11">
+        <v>712332</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" customHeight="1">
       <c r="A16" s="3">
         <v>11</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="B16" s="13">
+        <v>18</v>
+      </c>
+      <c r="C16" s="9">
+        <v>712117</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" ht="16.5" customHeight="1">
       <c r="A17" s="3">
         <v>12</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="14"/>
+      <c r="C17" s="11">
+        <v>712004</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" customHeight="1">
       <c r="A18" s="3">
         <v>13</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="B18" s="14"/>
+      <c r="C18" s="11">
+        <v>712055</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" ht="16.5" customHeight="1">
       <c r="A19" s="3">
         <v>14</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="B19" s="15"/>
+      <c r="C19" s="11">
+        <v>712118</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" ht="16.5" customHeight="1">
       <c r="A20" s="3">
         <v>15</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="13">
+        <v>19</v>
+      </c>
+      <c r="C20" s="9">
+        <v>712361</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1">
       <c r="A21" s="3">
         <v>16</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="B21" s="14">
+        <v>19</v>
+      </c>
+      <c r="C21" s="11">
+        <v>712429</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" ht="16.5" customHeight="1">
       <c r="A22" s="3">
         <v>17</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="B22" s="14"/>
+      <c r="C22" s="11">
+        <v>712467</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" ht="16.5" customHeight="1">
       <c r="A23" s="3">
         <v>18</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="B23" s="14"/>
+      <c r="C23" s="11">
+        <v>712151</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" ht="16.5" customHeight="1">
       <c r="A24" s="3">
         <v>19</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="B24" s="15"/>
+      <c r="C24" s="11">
+        <v>712452</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" customHeight="1">
       <c r="A25" s="3">
         <v>20</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="B25" s="13">
+        <v>20</v>
+      </c>
+      <c r="C25" s="9">
+        <v>712367</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" ht="16.5" customHeight="1">
       <c r="A26" s="3">
         <v>21</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="B26" s="14">
+        <v>20</v>
+      </c>
+      <c r="C26" s="11">
+        <v>712006</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" ht="16.5" customHeight="1">
       <c r="A27" s="3">
         <v>22</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="B27" s="14"/>
+      <c r="C27" s="11">
+        <v>712095</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" ht="16.5" customHeight="1">
       <c r="A28" s="3">
         <v>23</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="14"/>
+      <c r="C28" s="11">
+        <v>712065</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" ht="16.5" customHeight="1">
       <c r="A29" s="3">
         <v>24</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="3">
-        <v>25</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
+      <c r="B29" s="15"/>
+      <c r="C29" s="11">
+        <v>712091</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" ht="16.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:E3"/>
+  <mergeCells count="6">
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A2:F3"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B16:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Thêm kế hoạch Iteration 3. Đánh giá nhóm 17.
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -272,62 +272,62 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -642,71 +642,71 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="5" spans="1:15" s="21" customFormat="1" ht="33" customHeight="1">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:15" s="17" customFormat="1" ht="33" customHeight="1">
+      <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -714,13 +714,13 @@
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="19">
         <v>16</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>712312</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3">
@@ -742,11 +742,11 @@
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="7">
+      <c r="B7" s="20"/>
+      <c r="C7" s="6">
         <v>712308</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="3">
@@ -768,11 +768,11 @@
       <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7">
+      <c r="B8" s="20"/>
+      <c r="C8" s="6">
         <v>712303</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3">
@@ -794,11 +794,11 @@
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="7">
+      <c r="B9" s="20"/>
+      <c r="C9" s="6">
         <v>712181</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="3">
@@ -820,11 +820,11 @@
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="7">
+      <c r="B10" s="21"/>
+      <c r="C10" s="6">
         <v>712372</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="3">
@@ -846,20 +846,22 @@
       <c r="A11" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="19">
         <v>17</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>712255</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F11" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -874,18 +876,20 @@
       <c r="A12" s="3">
         <v>7</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="11">
+      <c r="B12" s="20"/>
+      <c r="C12" s="10">
         <v>712229</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -900,18 +904,20 @@
       <c r="A13" s="3">
         <v>8</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="11">
+      <c r="B13" s="20"/>
+      <c r="C13" s="10">
         <v>712201</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -926,18 +932,20 @@
       <c r="A14" s="3">
         <v>9</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="11">
+      <c r="B14" s="20"/>
+      <c r="C14" s="10">
         <v>712314</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -952,18 +960,20 @@
       <c r="A15" s="3">
         <v>10</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="11">
+      <c r="B15" s="21"/>
+      <c r="C15" s="10">
         <v>712332</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -978,13 +988,13 @@
       <c r="A16" s="3">
         <v>11</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="19">
         <v>18</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>712117</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="3">
@@ -1006,11 +1016,11 @@
       <c r="A17" s="3">
         <v>12</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11">
+      <c r="B17" s="20"/>
+      <c r="C17" s="10">
         <v>712004</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="3">
@@ -1032,11 +1042,11 @@
       <c r="A18" s="3">
         <v>13</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11">
+      <c r="B18" s="20"/>
+      <c r="C18" s="10">
         <v>712055</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="3">
@@ -1058,11 +1068,11 @@
       <c r="A19" s="3">
         <v>14</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="11">
+      <c r="B19" s="21"/>
+      <c r="C19" s="10">
         <v>712118</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="3">
@@ -1084,13 +1094,13 @@
       <c r="A20" s="3">
         <v>15</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="19">
         <v>19</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>712361</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="3">
@@ -1112,13 +1122,13 @@
       <c r="A21" s="3">
         <v>16</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="20">
         <v>19</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>712429</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="3">
@@ -1140,11 +1150,11 @@
       <c r="A22" s="3">
         <v>17</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11">
+      <c r="B22" s="20"/>
+      <c r="C22" s="10">
         <v>712467</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="3">
@@ -1166,11 +1176,11 @@
       <c r="A23" s="3">
         <v>18</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="11">
+      <c r="B23" s="20"/>
+      <c r="C23" s="10">
         <v>712151</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="3">
@@ -1192,11 +1202,11 @@
       <c r="A24" s="3">
         <v>19</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="11">
+      <c r="B24" s="21"/>
+      <c r="C24" s="10">
         <v>712452</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="3">
@@ -1218,13 +1228,13 @@
       <c r="A25" s="3">
         <v>20</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="19">
         <v>20</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>712367</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="3">
@@ -1246,13 +1256,13 @@
       <c r="A26" s="3">
         <v>21</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="20">
         <v>20</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>712006</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="3">
@@ -1274,11 +1284,11 @@
       <c r="A27" s="3">
         <v>22</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="11">
+      <c r="B27" s="20"/>
+      <c r="C27" s="10">
         <v>712095</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E27" s="3">
@@ -1300,11 +1310,11 @@
       <c r="A28" s="3">
         <v>23</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="11">
+      <c r="B28" s="20"/>
+      <c r="C28" s="10">
         <v>712065</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="3">
@@ -1326,11 +1336,11 @@
       <c r="A29" s="3">
         <v>24</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="11">
+      <c r="B29" s="21"/>
+      <c r="C29" s="10">
         <v>712091</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="3">

</xml_diff>

<commit_message>
[10-05]Đánh giá nhóm 17.
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -108,19 +108,10 @@
     <t>Nhóm</t>
   </si>
   <si>
-    <t>ĐG lần 3</t>
-  </si>
-  <si>
-    <t>ĐG lần 4</t>
-  </si>
-  <si>
     <t>ĐG lần 
 (05/05)</t>
   </si>
   <si>
-    <t>ĐG lần 5</t>
-  </si>
-  <si>
     <t>ĐG lần 6</t>
   </si>
   <si>
@@ -141,6 +132,18 @@
   <si>
     <t>ĐG lần 2
 (10/05)</t>
+  </si>
+  <si>
+    <t>ĐG lần 3
+(13/05)</t>
+  </si>
+  <si>
+    <t>ĐG lần 4
+(17/05)</t>
+  </si>
+  <si>
+    <t>ĐG lần 5
+(20/05)</t>
   </si>
 </sst>
 </file>
@@ -636,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -676,7 +679,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="33" customHeight="1">
@@ -696,34 +699,34 @@
         <v>28</v>
       </c>
       <c r="F5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="N5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="O5" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1">
@@ -873,12 +876,14 @@
       </c>
       <c r="E11" s="19">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -901,12 +906,14 @@
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -929,12 +936,14 @@
       </c>
       <c r="E13" s="19">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -957,12 +966,14 @@
       </c>
       <c r="E14" s="19">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -985,12 +996,14 @@
       </c>
       <c r="E15" s="19">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>

</xml_diff>

<commit_message>
Chức năng chính tả gần hoàn thiện
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -904,7 +904,9 @@
       <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -934,7 +936,9 @@
       <c r="G12" s="3">
         <v>1</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -964,7 +968,9 @@
       <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -986,7 +992,7 @@
       </c>
       <c r="E14" s="19">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -994,7 +1000,9 @@
       <c r="G14" s="3">
         <v>1</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1024,7 +1032,9 @@
       <c r="G15" s="3">
         <v>1</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>

</xml_diff>

<commit_message>
Thêm Release100520.rar Thêm kế hoạch Iteration 5
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -112,9 +112,6 @@
 (05/05)</t>
   </si>
   <si>
-    <t>ĐG lần 6</t>
-  </si>
-  <si>
     <t>ĐG lần 7</t>
   </si>
   <si>
@@ -144,6 +141,10 @@
   <si>
     <t>ĐG lần 5
 (20/05)</t>
+  </si>
+  <si>
+    <t>ĐG lần 6
+(24/05)</t>
   </si>
 </sst>
 </file>
@@ -157,7 +158,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -177,13 +178,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -639,20 +640,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="1" customWidth="1"/>
-    <col min="6" max="14" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.125" style="1"/>
+    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="14" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15">
@@ -679,7 +680,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="33" customHeight="1">
@@ -702,31 +703,31 @@
         <v>30</v>
       </c>
       <c r="G5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="I5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="K5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="N5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="O5" s="16" t="s">
         <v>34</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1">
@@ -896,7 +897,7 @@
       </c>
       <c r="E11" s="19">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -910,7 +911,9 @@
       <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -930,7 +933,7 @@
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -944,7 +947,9 @@
       <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -978,7 +983,9 @@
       <c r="I13" s="3">
         <v>0</v>
       </c>
-      <c r="J13" s="3"/>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -998,7 +1005,7 @@
       </c>
       <c r="E14" s="19">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -1012,7 +1019,9 @@
       <c r="I14" s="3">
         <v>1</v>
       </c>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1046,7 +1055,9 @@
       <c r="I15" s="3">
         <v>0</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -1562,7 +1573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1574,7 +1585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Group18] Danh Gia Thanh Vien Lan 6
</commit_message>
<xml_diff>
--- a/BangVangThanhTich.xlsx
+++ b/BangVangThanhTich.xlsx
@@ -641,7 +641,7 @@
   <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="E16" s="19">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
@@ -1096,7 +1096,9 @@
       <c r="J16" s="3">
         <v>0</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1115,7 +1117,7 @@
       </c>
       <c r="E17" s="19">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -1132,7 +1134,9 @@
       <c r="J17" s="3">
         <v>1</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1151,7 +1155,7 @@
       </c>
       <c r="E18" s="19">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -1168,7 +1172,9 @@
       <c r="J18" s="3">
         <v>1</v>
       </c>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1187,7 +1193,7 @@
       </c>
       <c r="E19" s="19">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -1204,7 +1210,9 @@
       <c r="J19" s="3">
         <v>1</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>

</xml_diff>